<commit_message>
can configure location and when reports are generated in input file
</commit_message>
<xml_diff>
--- a/end_of_day_reports_input.xlsx
+++ b/end_of_day_reports_input.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11970"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11970" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
-    <sheet name="who_dummies" sheetId="2" r:id="rId2"/>
+    <sheet name="report_locations" sheetId="3" r:id="rId2"/>
+    <sheet name="who_dummies" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="370">
   <si>
     <t>report</t>
   </si>
@@ -1093,6 +1094,48 @@
   </si>
   <si>
     <t>Canada</t>
+  </si>
+  <si>
+    <t>dir</t>
+  </si>
+  <si>
+    <t>C:/Users/hswerdfe/Documents/reports/qry</t>
+  </si>
+  <si>
+    <t>C:/Users/hswerdfe/Documents/reports/DS</t>
+  </si>
+  <si>
+    <t>C:/Users/hswerdfe/Documents/reports/HC</t>
+  </si>
+  <si>
+    <t>C:/Users/hswerdfe/Documents/reports/STAT</t>
+  </si>
+  <si>
+    <t>C:/Users/hswerdfe/Documents/reports/WHO</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Sun</t>
+  </si>
+  <si>
+    <t>Mon</t>
+  </si>
+  <si>
+    <t>Tue</t>
+  </si>
+  <si>
+    <t>Wed</t>
+  </si>
+  <si>
+    <t>Thu</t>
+  </si>
+  <si>
+    <t>Fri</t>
+  </si>
+  <si>
+    <t>Sat</t>
   </si>
 </sst>
 </file>
@@ -1412,8 +1455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B408"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A280" workbookViewId="0">
+      <selection activeCell="B284" sqref="B284:B291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4693,6 +4736,199 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C1" t="s">
+        <v>363</v>
+      </c>
+      <c r="D1" t="s">
+        <v>364</v>
+      </c>
+      <c r="E1" t="s">
+        <v>365</v>
+      </c>
+      <c r="F1" t="s">
+        <v>366</v>
+      </c>
+      <c r="G1" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1" t="s">
+        <v>368</v>
+      </c>
+      <c r="I1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D2" t="s">
+        <v>362</v>
+      </c>
+      <c r="E2" t="s">
+        <v>362</v>
+      </c>
+      <c r="F2" t="s">
+        <v>362</v>
+      </c>
+      <c r="G2" t="s">
+        <v>362</v>
+      </c>
+      <c r="H2" t="s">
+        <v>362</v>
+      </c>
+      <c r="I2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C3" t="s">
+        <v>362</v>
+      </c>
+      <c r="D3" t="s">
+        <v>362</v>
+      </c>
+      <c r="E3" t="s">
+        <v>362</v>
+      </c>
+      <c r="F3" t="s">
+        <v>362</v>
+      </c>
+      <c r="G3" t="s">
+        <v>362</v>
+      </c>
+      <c r="H3" t="s">
+        <v>362</v>
+      </c>
+      <c r="I3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B4" t="s">
+        <v>359</v>
+      </c>
+      <c r="C4" t="s">
+        <v>362</v>
+      </c>
+      <c r="D4" t="s">
+        <v>362</v>
+      </c>
+      <c r="E4" t="s">
+        <v>362</v>
+      </c>
+      <c r="F4" t="s">
+        <v>362</v>
+      </c>
+      <c r="G4" t="s">
+        <v>362</v>
+      </c>
+      <c r="H4" t="s">
+        <v>362</v>
+      </c>
+      <c r="I4" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>225</v>
+      </c>
+      <c r="B5" t="s">
+        <v>360</v>
+      </c>
+      <c r="C5" t="s">
+        <v>362</v>
+      </c>
+      <c r="D5" t="s">
+        <v>362</v>
+      </c>
+      <c r="E5" t="s">
+        <v>362</v>
+      </c>
+      <c r="F5" t="s">
+        <v>362</v>
+      </c>
+      <c r="G5" t="s">
+        <v>362</v>
+      </c>
+      <c r="H5" t="s">
+        <v>362</v>
+      </c>
+      <c r="I5" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>351</v>
+      </c>
+      <c r="B6" t="s">
+        <v>361</v>
+      </c>
+      <c r="C6" t="s">
+        <v>362</v>
+      </c>
+      <c r="D6" t="s">
+        <v>362</v>
+      </c>
+      <c r="E6" t="s">
+        <v>362</v>
+      </c>
+      <c r="F6" t="s">
+        <v>362</v>
+      </c>
+      <c r="G6" t="s">
+        <v>362</v>
+      </c>
+      <c r="H6" t="s">
+        <v>362</v>
+      </c>
+      <c r="I6" t="s">
+        <v>362</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>

</xml_diff>

<commit_message>
produces db error report now, for cases that look strange.
</commit_message>
<xml_diff>
--- a/end_of_day_reports_input.xlsx
+++ b/end_of_day_reports_input.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="372">
   <si>
     <t>report</t>
   </si>
@@ -1136,6 +1136,12 @@
   </si>
   <si>
     <t>~/covid_case_reports/qry</t>
+  </si>
+  <si>
+    <t>~/covid_case_reports/db_errs</t>
+  </si>
+  <si>
+    <t>db_errs</t>
   </si>
 </sst>
 </file>
@@ -4737,10 +4743,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4920,6 +4926,35 @@
         <v>357</v>
       </c>
       <c r="I6" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>371</v>
+      </c>
+      <c r="B7" t="s">
+        <v>370</v>
+      </c>
+      <c r="C7" t="s">
+        <v>357</v>
+      </c>
+      <c r="D7" t="s">
+        <v>357</v>
+      </c>
+      <c r="E7" t="s">
+        <v>357</v>
+      </c>
+      <c r="F7" t="s">
+        <v>357</v>
+      </c>
+      <c r="G7" t="s">
+        <v>357</v>
+      </c>
+      <c r="H7" t="s">
+        <v>357</v>
+      </c>
+      <c r="I7" t="s">
         <v>357</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reports now call the query, and the postfix on the name is gone.
</commit_message>
<xml_diff>
--- a/end_of_day_reports_input.xlsx
+++ b/end_of_day_reports_input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11970"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11970" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1653" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="418">
   <si>
     <t>report</t>
   </si>
@@ -1260,13 +1260,37 @@
   </si>
   <si>
     <t>Occupation_other</t>
+  </si>
+  <si>
+    <t>//Ncr-a_irbv2s/irbv2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DATABASE/MS ACCESS/OUTPUT/percent_time</t>
+  </si>
+  <si>
+    <t>percent_by_time</t>
+  </si>
+  <si>
+    <t>ETHNICITY</t>
+  </si>
+  <si>
+    <t>Ethnicity</t>
+  </si>
+  <si>
+    <t>ASYMPTOMATIC</t>
+  </si>
+  <si>
+    <t>Current Outcome</t>
+  </si>
+  <si>
+    <t>ijn</t>
+  </si>
+  <si>
+    <t>\\Ncr-a_irbv2s\irbv2\PHAC\IDPCB\CIRID\VIPS-SAR\EMERGENCY PREPAREDNESS AND RESPONSE HC4\EMERGENCY EVENT\WUHAN UNKNOWN PNEU - 2020\DATA AND ANALYSIS\CANADA CASE REPORTS\IJN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1287,6 +1311,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1310,13 +1340,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1600,8 +1631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C508"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7208,10 +7239,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7346,24 +7377,6 @@
       <c r="C5" t="s">
         <v>357</v>
       </c>
-      <c r="D5" t="s">
-        <v>357</v>
-      </c>
-      <c r="E5" t="s">
-        <v>357</v>
-      </c>
-      <c r="F5" t="s">
-        <v>357</v>
-      </c>
-      <c r="G5" t="s">
-        <v>357</v>
-      </c>
-      <c r="H5" t="s">
-        <v>357</v>
-      </c>
-      <c r="I5" t="s">
-        <v>357</v>
-      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -7507,6 +7520,64 @@
         <v>357</v>
       </c>
       <c r="I10" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>411</v>
+      </c>
+      <c r="B11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C11" t="s">
+        <v>357</v>
+      </c>
+      <c r="D11" t="s">
+        <v>357</v>
+      </c>
+      <c r="E11" t="s">
+        <v>357</v>
+      </c>
+      <c r="F11" t="s">
+        <v>357</v>
+      </c>
+      <c r="G11" t="s">
+        <v>357</v>
+      </c>
+      <c r="H11" t="s">
+        <v>357</v>
+      </c>
+      <c r="I11" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>416</v>
+      </c>
+      <c r="B12" t="s">
+        <v>417</v>
+      </c>
+      <c r="C12" t="s">
+        <v>357</v>
+      </c>
+      <c r="D12" t="s">
+        <v>357</v>
+      </c>
+      <c r="E12" t="s">
+        <v>357</v>
+      </c>
+      <c r="F12" t="s">
+        <v>357</v>
+      </c>
+      <c r="G12" t="s">
+        <v>357</v>
+      </c>
+      <c r="H12" t="s">
+        <v>357</v>
+      </c>
+      <c r="I12" t="s">
         <v>357</v>
       </c>
     </row>
@@ -7518,18 +7589,19 @@
     <hyperlink ref="B2" r:id="rId4" display="\\Ncr-a_irbv2s\irbv2\PHAC\IDPCB\CIRID\VIPS-SAR\EMERGENCY PREPAREDNESS AND RESPONSE HC4\EMERGENCY EVENT\WUHAN UNKNOWN PNEU - 2020\DATA AND ANALYSIS\DATABASE\MS ACCESS\OUTPUT/qry"/>
     <hyperlink ref="B3" r:id="rId5" display="\\Ncr-a_irbv2s\irbv2\PHAC\IDPCB\CIRID\VIPS-SAR\EMERGENCY PREPAREDNESS AND RESPONSE HC4\EMERGENCY EVENT\WUHAN UNKNOWN PNEU - 2020\DATA AND ANALYSIS\PHAC MODELLING\Domestic data"/>
     <hyperlink ref="B10" r:id="rId6" display="\\Ncr-a_irbv2s\irbv2\PHAC\IDPCB\CIRID\VIPS-SAR\EMERGENCY PREPAREDNESS AND RESPONSE HC4\EMERGENCY EVENT\WUHAN UNKNOWN PNEU - 2020\DATA AND ANALYSIS\DATABASE\MS ACCESS\OUTPUT/by_age_prov"/>
+    <hyperlink ref="B11" r:id="rId7" display="\\Ncr-a_irbv2s\irbv2\PHAC\IDPCB\CIRID\VIPS-SAR\EMERGENCY PREPAREDNESS AND RESPONSE HC4\EMERGENCY EVENT\WUHAN UNKNOWN PNEU - 2020\DATA AND ANALYSIS\DATABASE\MS ACCESS\OUTPUT/epi_curves"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7648,8 +7720,33 @@
         <v>393</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="B12" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" t="s">
+        <v>415</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
lower case for column names and configure file for values
</commit_message>
<xml_diff>
--- a/end_of_day_reports_input.xlsx
+++ b/end_of_day_reports_input.xlsx
@@ -1670,8 +1670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F508"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" topLeftCell="A313" workbookViewId="0">
+      <selection activeCell="D322" sqref="D322"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3575,7 +3575,7 @@
         <v>383</v>
       </c>
       <c r="D95" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E95" t="s">
         <v>429</v>
@@ -11856,7 +11856,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
change to datahub report and to counts summary report and to column ordering now works again on all reports
</commit_message>
<xml_diff>
--- a/end_of_day_reports_input.xlsx
+++ b/end_of_day_reports_input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11970" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11970"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="who_dummies" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">input!$A$1:$F$534</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">input!$A$1:$F$536</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3389" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3401" uniqueCount="442">
   <si>
     <t>report</t>
   </si>
@@ -1350,6 +1350,12 @@
   </si>
   <si>
     <t>exposure_cat</t>
+  </si>
+  <si>
+    <t>EpisodeDate_imputed</t>
+  </si>
+  <si>
+    <t>OnsetDate_imputed</t>
   </si>
 </sst>
 </file>
@@ -1695,10 +1701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F534"/>
+  <dimension ref="A1:F536"/>
   <sheetViews>
-    <sheetView topLeftCell="A501" workbookViewId="0">
-      <selection activeCell="A508" sqref="A508"/>
+    <sheetView tabSelected="1" topLeftCell="A501" workbookViewId="0">
+      <selection activeCell="B507" sqref="B507"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11792,7 +11798,7 @@
         <v>4</v>
       </c>
       <c r="C506" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E506" t="s">
         <v>410</v>
@@ -11818,7 +11824,7 @@
         <v>410</v>
       </c>
       <c r="F507" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
     </row>
     <row r="508" spans="1:6" x14ac:dyDescent="0.25">
@@ -11826,13 +11832,13 @@
         <v>428</v>
       </c>
       <c r="B508" t="s">
-        <v>12</v>
+        <v>440</v>
       </c>
       <c r="C508" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D508" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E508" t="s">
         <v>410</v>
@@ -11846,7 +11852,7 @@
         <v>428</v>
       </c>
       <c r="B509" t="s">
-        <v>429</v>
+        <v>12</v>
       </c>
       <c r="C509" t="s">
         <v>380</v>
@@ -11866,7 +11872,7 @@
         <v>428</v>
       </c>
       <c r="B510" t="s">
-        <v>383</v>
+        <v>429</v>
       </c>
       <c r="C510" t="s">
         <v>380</v>
@@ -11886,7 +11892,7 @@
         <v>428</v>
       </c>
       <c r="B511" t="s">
-        <v>18</v>
+        <v>383</v>
       </c>
       <c r="C511" t="s">
         <v>380</v>
@@ -11906,7 +11912,7 @@
         <v>428</v>
       </c>
       <c r="B512" t="s">
-        <v>212</v>
+        <v>18</v>
       </c>
       <c r="C512" t="s">
         <v>380</v>
@@ -11926,7 +11932,7 @@
         <v>428</v>
       </c>
       <c r="B513" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C513" t="s">
         <v>380</v>
@@ -11946,7 +11952,7 @@
         <v>428</v>
       </c>
       <c r="B514" t="s">
-        <v>25</v>
+        <v>213</v>
       </c>
       <c r="C514" t="s">
         <v>380</v>
@@ -11966,7 +11972,7 @@
         <v>428</v>
       </c>
       <c r="B515" t="s">
-        <v>198</v>
+        <v>25</v>
       </c>
       <c r="C515" t="s">
         <v>380</v>
@@ -11986,19 +11992,19 @@
         <v>428</v>
       </c>
       <c r="B516" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="C516" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D516" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="E516" t="s">
         <v>410</v>
       </c>
       <c r="F516" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
     </row>
     <row r="517" spans="1:6" x14ac:dyDescent="0.25">
@@ -12006,13 +12012,13 @@
         <v>428</v>
       </c>
       <c r="B517" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C517" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D517" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E517" t="s">
         <v>410</v>
@@ -12026,13 +12032,13 @@
         <v>428</v>
       </c>
       <c r="B518" t="s">
-        <v>31</v>
+        <v>441</v>
       </c>
       <c r="C518" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D518" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E518" t="s">
         <v>410</v>
@@ -12046,7 +12052,7 @@
         <v>428</v>
       </c>
       <c r="B519" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C519" t="s">
         <v>380</v>
@@ -12066,7 +12072,7 @@
         <v>428</v>
       </c>
       <c r="B520" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C520" t="s">
         <v>380</v>
@@ -12086,7 +12092,7 @@
         <v>428</v>
       </c>
       <c r="B521" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C521" t="s">
         <v>380</v>
@@ -12106,7 +12112,7 @@
         <v>428</v>
       </c>
       <c r="B522" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C522" t="s">
         <v>380</v>
@@ -12126,7 +12132,7 @@
         <v>428</v>
       </c>
       <c r="B523" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C523" t="s">
         <v>380</v>
@@ -12146,7 +12152,7 @@
         <v>428</v>
       </c>
       <c r="B524" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C524" t="s">
         <v>380</v>
@@ -12166,7 +12172,7 @@
         <v>428</v>
       </c>
       <c r="B525" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C525" t="s">
         <v>380</v>
@@ -12186,7 +12192,7 @@
         <v>428</v>
       </c>
       <c r="B526" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C526" t="s">
         <v>380</v>
@@ -12206,7 +12212,7 @@
         <v>428</v>
       </c>
       <c r="B527" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C527" t="s">
         <v>380</v>
@@ -12226,7 +12232,7 @@
         <v>428</v>
       </c>
       <c r="B528" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C528" t="s">
         <v>380</v>
@@ -12246,7 +12252,7 @@
         <v>428</v>
       </c>
       <c r="B529" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C529" t="s">
         <v>380</v>
@@ -12266,13 +12272,13 @@
         <v>428</v>
       </c>
       <c r="B530" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C530" t="s">
         <v>380</v>
       </c>
       <c r="D530" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="E530" t="s">
         <v>410</v>
@@ -12286,10 +12292,13 @@
         <v>428</v>
       </c>
       <c r="B531" t="s">
-        <v>216</v>
+        <v>42</v>
       </c>
       <c r="C531" t="s">
         <v>380</v>
+      </c>
+      <c r="D531" t="s">
+        <v>407</v>
       </c>
       <c r="E531" t="s">
         <v>410</v>
@@ -12303,13 +12312,13 @@
         <v>428</v>
       </c>
       <c r="B532" t="s">
-        <v>217</v>
+        <v>43</v>
       </c>
       <c r="C532" t="s">
         <v>380</v>
       </c>
       <c r="D532" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E532" t="s">
         <v>410</v>
@@ -12323,19 +12332,16 @@
         <v>428</v>
       </c>
       <c r="B533" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C533" t="s">
-        <v>381</v>
-      </c>
-      <c r="D533" t="s">
-        <v>406</v>
+        <v>380</v>
       </c>
       <c r="E533" t="s">
         <v>410</v>
       </c>
       <c r="F533" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
     </row>
     <row r="534" spans="1:6" x14ac:dyDescent="0.25">
@@ -12343,23 +12349,63 @@
         <v>428</v>
       </c>
       <c r="B534" t="s">
+        <v>217</v>
+      </c>
+      <c r="C534" t="s">
+        <v>380</v>
+      </c>
+      <c r="D534" t="s">
+        <v>407</v>
+      </c>
+      <c r="E534" t="s">
+        <v>410</v>
+      </c>
+      <c r="F534" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="535" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A535" t="s">
+        <v>428</v>
+      </c>
+      <c r="B535" t="s">
+        <v>218</v>
+      </c>
+      <c r="C535" t="s">
+        <v>381</v>
+      </c>
+      <c r="D535" t="s">
+        <v>406</v>
+      </c>
+      <c r="E535" t="s">
+        <v>410</v>
+      </c>
+      <c r="F535" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="536" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A536" t="s">
+        <v>428</v>
+      </c>
+      <c r="B536" t="s">
         <v>219</v>
       </c>
-      <c r="C534" t="s">
-        <v>380</v>
-      </c>
-      <c r="D534" t="s">
-        <v>407</v>
-      </c>
-      <c r="E534" t="s">
-        <v>410</v>
-      </c>
-      <c r="F534" t="s">
+      <c r="C536" t="s">
+        <v>380</v>
+      </c>
+      <c r="D536" t="s">
+        <v>407</v>
+      </c>
+      <c r="E536" t="s">
+        <v>410</v>
+      </c>
+      <c r="F536" t="s">
         <v>401</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F534"/>
+  <autoFilter ref="A1:F536"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -12865,8 +12911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
all metabase extracts in one spot.
</commit_message>
<xml_diff>
--- a/end_of_day_reports_input.xlsx
+++ b/end_of_day_reports_input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SCONNORS\Desktop\covid_cases_data_extracts-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hswerdfe\Documents\Projects\covid_cases_data_extracts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3372" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3405" uniqueCount="444">
   <si>
     <t>report</t>
   </si>
@@ -1359,6 +1359,18 @@
   </si>
   <si>
     <t>L:/HPOC/Active Events/001-20 COVID-19/Operations/Surveillance - Epi. Diagnostics/Canada_COVID19_WHO_linelist</t>
+  </si>
+  <si>
+    <t>static_file</t>
+  </si>
+  <si>
+    <t>static_file_web</t>
+  </si>
+  <si>
+    <t>//Ncr-a_irbv2s/irbv2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DASHBOARD</t>
+  </si>
+  <si>
+    <t>//Ncr-a_irbv2s/irbv2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DATABASE</t>
   </si>
 </sst>
 </file>
@@ -12345,8 +12357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12506,6 +12518,24 @@
       <c r="D5" t="s">
         <v>381</v>
       </c>
+      <c r="E5" t="s">
+        <v>381</v>
+      </c>
+      <c r="F5" t="s">
+        <v>381</v>
+      </c>
+      <c r="G5" t="s">
+        <v>381</v>
+      </c>
+      <c r="H5" t="s">
+        <v>381</v>
+      </c>
+      <c r="I5" t="s">
+        <v>381</v>
+      </c>
+      <c r="J5" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -12517,7 +12547,25 @@
       <c r="C6" t="s">
         <v>387</v>
       </c>
+      <c r="D6" t="s">
+        <v>381</v>
+      </c>
+      <c r="E6" t="s">
+        <v>381</v>
+      </c>
+      <c r="F6" t="s">
+        <v>381</v>
+      </c>
+      <c r="G6" t="s">
+        <v>381</v>
+      </c>
       <c r="H6" t="s">
+        <v>381</v>
+      </c>
+      <c r="I6" t="s">
+        <v>381</v>
+      </c>
+      <c r="J6" t="s">
         <v>381</v>
       </c>
       <c r="K6" t="s">
@@ -12812,7 +12860,71 @@
         <v>381</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>440</v>
+      </c>
+      <c r="B16" t="s">
+        <v>379</v>
+      </c>
+      <c r="C16" t="s">
+        <v>442</v>
+      </c>
+      <c r="D16" t="s">
+        <v>381</v>
+      </c>
+      <c r="E16" t="s">
+        <v>381</v>
+      </c>
+      <c r="F16" t="s">
+        <v>381</v>
+      </c>
+      <c r="G16" t="s">
+        <v>381</v>
+      </c>
+      <c r="H16" t="s">
+        <v>381</v>
+      </c>
+      <c r="I16" t="s">
+        <v>381</v>
+      </c>
+      <c r="J16" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>441</v>
+      </c>
+      <c r="B17" t="s">
+        <v>379</v>
+      </c>
+      <c r="C17" t="s">
+        <v>443</v>
+      </c>
+      <c r="D17" t="s">
+        <v>381</v>
+      </c>
+      <c r="E17" t="s">
+        <v>381</v>
+      </c>
+      <c r="F17" t="s">
+        <v>381</v>
+      </c>
+      <c r="G17" t="s">
+        <v>381</v>
+      </c>
+      <c r="H17" t="s">
+        <v>381</v>
+      </c>
+      <c r="I17" t="s">
+        <v>381</v>
+      </c>
+      <c r="J17" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
     </row>
   </sheetData>

</xml_diff>